<commit_message>
changed haplotype to microhaplotype;
</commit_message>
<xml_diff>
--- a/project/excel/portable_microhaplotype_object.xlsx
+++ b/project/excel/portable_microhaplotype_object.xlsx
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="TargetInfo" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="PanelInfo" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RepresentativeHaplotypeSequence" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="RepresentativeHaplotypeSequences" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="HaplotypesDetected" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="RepresentativeMicrohaplotypeSequence" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="RepresentativeMicrohaplotypeSequences" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MicrohaplotypesDetected" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="DemultiplexedSamples" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="DemultiplexedTargetsForSample" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="DemultiplexedTargetForSample" sheetId="8" state="visible" r:id="rId8"/>
@@ -19,9 +19,9 @@
     <sheet name="GenomicLocation" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="PrimerInfo" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Primers" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="HaplotypesForSample" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="HaplotypeForTarget" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="HaplotypesForTarget" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="MicrohaplotypesForSample" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="MicrohaplotypeForTarget" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="MicrohaplotypesForTarget" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="TarAmpBioinformaticsInfo" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="BioMethod" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="SequencingInfo" sheetId="18" state="visible" r:id="rId18"/>
@@ -618,7 +618,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>haplotype_id</t>
+          <t>microhaplotype_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>haplotypes</t>
+          <t>microhaplotypes</t>
         </is>
       </c>
     </row>
@@ -1005,12 +1005,12 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>representative_haplotype_sequences</t>
+          <t>representative_microhaplotype_sequences</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>haplotypes_detected</t>
+          <t>microhaplotypes_detected</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>haplotype_id</t>
+          <t>microhaplotype_id</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">

</xml_diff>

<commit_message>
modifications to the IDs; added ExperimentInfo;
</commit_message>
<xml_diff>
--- a/project/excel/portable_microhaplotype_object.xlsx
+++ b/project/excel/portable_microhaplotype_object.xlsx
@@ -24,9 +24,10 @@
     <sheet name="MicrohaplotypesForTarget" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="TarAmpBioinformaticsInfo" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="BioMethod" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="SequencingInfo" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="SpecimenInfo" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="PortableMicrohaplotypeObject" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="ExperimentInfo" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="SequencingInfo" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SpecimenInfo" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="PortableMicrohaplotypeObject" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -587,7 +588,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>sample_id</t>
+          <t>experiment_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -761,7 +762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,6 +778,62 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>plate_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>plate_row</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>plate_col</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>specimen_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>panel_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>experiment_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequencing_info_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>seq_instrument</t>
         </is>
       </c>
@@ -797,142 +854,326 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>nucl_acid_date</t>
+          <t>nucl_acid_ext_date</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>nucl_acid_amp_date</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>pcr_cond</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>lib_screen</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>lib_layout</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>lib_kit</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>seq_center</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>panel_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>target_genome</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>targets</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>specimen_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>plate_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>plate_row</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>plate_col</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>samp_taxon_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>individual_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>host_taxon_id</t>
+        </is>
+      </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>lib_screen</t>
+          <t>alternate_identifiers</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>lib_layout</t>
+          <t>parasite_density</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>lib_kit</t>
+          <t>collection_date</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>seq_center</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sample_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>samp_taxon_id</t>
+          <t>lat_lon</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>geo_loc_name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>collector</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>samp_store_loc</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>samp_collect_device</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>accession</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>sample_comments</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>experiment_infos</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>specimen_infos</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>host_taxon_id</t>
+          <t>sequencing_info</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>alternate_identifiers</t>
+          <t>bioinformatics_info</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>parasite_density</t>
+          <t>panel_info</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>collection_date</t>
+          <t>representative_microhaplotype_sequences</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>lat_lon</t>
+          <t>microhaplotypes_detected</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>collector</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>samp_store_loc</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>samp_collect_device</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>project_name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>accession</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>sample_comments</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>plate_name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>plate_row</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>plate_col</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>target_demultiplexed_samples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>seq</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>microhaplotype_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>quality</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>alt_annotations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>target_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>seqs</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -949,314 +1190,150 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>panel_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>target_genome</t>
+          <t>sequencing_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bioinformatics_id</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>targets</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>specimen_infos</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequencing_info</t>
+          <t>samples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>demultiplexed_samples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>experiment_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>demultiplexed_targets</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>target_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>raw_read_count</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>bioinformatics_info</t>
+          <t>taxon_id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>panel_info</t>
+          <t>url</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>representative_microhaplotype_sequences</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>microhaplotypes_detected</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>target_demultiplexed_samples</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>seq</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>microhaplotype_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>quality</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>alt_annotations</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>target_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>seqs</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequencing_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bioinformatics_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>samples</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>demultiplexed_samples</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sample_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>demultiplexed_targets</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>target_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>raw_read_count</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>taxon_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
           <t>gff_url</t>
         </is>
       </c>

</xml_diff>

<commit_message>
added admin levels for geolocs
</commit_message>
<xml_diff>
--- a/project/excel/portable_microhaplotype_object.xlsx
+++ b/project/excel/portable_microhaplotype_object.xlsx
@@ -935,7 +935,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -996,40 +996,55 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>collection_country</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>geo_admin2</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>geo_admin3</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>lat_lon</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>geo_loc_name</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>collector</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>samp_store_loc</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>samp_collect_device</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>project_name</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>accession</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>sample_comments</t>
         </is>

</xml_diff>

<commit_message>
add bio id to the representative haplotypes;
</commit_message>
<xml_diff>
--- a/project/excel/portable_microhaplotype_object.xlsx
+++ b/project/excel/portable_microhaplotype_object.xlsx
@@ -12,22 +12,23 @@
     <sheet name="RepresentativeMicrohaplotypeSequence" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="MaskingInfo" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="RepresentativeMicrohaplotypeSequences" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="MicrohaplotypesDetected" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="DemultiplexedExperimentSamples" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="DemultiplexedTargetsForExperimentSample" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="DemultiplexedTargetForExperimentSample" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="GenomeInfo" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="GenomicLocation" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="PrimerInfo" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="MicrohaplotypesForSample" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="MicrohaplotypeForTarget" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="MicrohaplotypesForTarget" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="TarAmpBioinformaticsInfo" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="BioMethod" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="ExperimentInfo" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="SequencingInfo" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="SpecimenInfo" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="PortableMicrohaplotypeObject" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="RepresentativeMicrohaplotypesForTarget" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="MicrohaplotypesDetected" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="DemultiplexedExperimentSamples" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="DemultiplexedTargetsForExperimentSample" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="DemultiplexedTargetForExperimentSample" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="GenomeInfo" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="GenomicLocation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="PrimerInfo" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="MicrohaplotypesForSample" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="MicrohaplotypeForTarget" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="MicrohaplotypesForTarget" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="TarAmpBioinformaticsInfo" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="BioMethod" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="ExperimentInfo" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SequencingInfo" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="SpecimenInfo" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="PortableMicrohaplotypeObject" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -479,6 +480,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>target_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>raw_read_count</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -519,7 +551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -565,7 +597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -596,7 +628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -627,7 +659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -663,7 +695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -694,7 +726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -740,7 +772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -781,7 +813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -837,7 +869,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>panel_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>target_genome</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>panel_targets</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -918,33 +986,307 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>panel_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>target_genome</t>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>specimen_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>plate_name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>plate_row</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>plate_col</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>samp_taxon_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>individual_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>host_taxon_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alternate_identifiers</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>parasite_density</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>collection_date</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>collection_country</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>geo_admin2</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>geo_admin3</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>lat_lon</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>collector</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>samp_store_loc</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>samp_collect_device</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>accession</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>sample_comments</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>analysis_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>experiment_infos</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>specimen_infos</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sequencing_infos</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>panel_info</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>representative_microhaplotype_sequences</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>microhaplotypes_detected</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>target_demultiplexed_experiment_samples</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>taramp_bioinformatics_infos</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>postprocessing_bioinformatics_infos</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>seq</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>microhaplotype_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>quality</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pseudocigar</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>masking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>alt_annotations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>seq_start</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>segment_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>tar_amp_bioinformatics_info_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>targets</t>
         </is>
       </c>
@@ -954,255 +1296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>specimen_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>plate_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>plate_row</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>plate_col</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>samp_taxon_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>individual_id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>host_taxon_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>alternate_identifiers</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>parasite_density</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>collection_date</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>collection_country</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>geo_admin1</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>geo_admin2</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>geo_admin3</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>lat_lon</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>collector</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>samp_store_loc</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>samp_collect_device</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>project_name</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>accession</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>sample_comments</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>analysis_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>experiment_infos</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>specimen_infos</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sequencing_infos</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>panel_info</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>representative_microhaplotype_sequences</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>microhaplotypes_detected</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>target_demultiplexed_experiment_samples</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>taramp_bioinformatics_infos</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>postprocessing_bioinformatics_infos</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>seq</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>microhaplotype_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>quality</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>pseudocigar</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>masking</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>alt_annotations</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1219,21 +1313,21 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>seq_start</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>segment_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>target_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>seqs</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1250,21 +1344,21 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>target_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>seqs</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>tar_amp_bioinformatics_info_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>experiment_samples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1286,16 +1380,16 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>experiment_samples</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>demultiplexed_experiment_samples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1312,37 +1406,6 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>tar_amp_bioinformatics_info_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>demultiplexed_experiment_samples</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>experiment_sample_id</t>
         </is>
       </c>
@@ -1355,35 +1418,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>target_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>raw_read_count</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added project_info to store information about a project that specimens might belong to;
</commit_message>
<xml_diff>
--- a/project/excel/portable_microhaplotype_object.xlsx
+++ b/project/excel/portable_microhaplotype_object.xlsx
@@ -28,15 +28,16 @@
     <sheet name="ExperimentInfo" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="SequencingInfo" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="ParasiteDensity" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="SpecimenInfo" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="BioinformaticsRunInfo" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="PmoGenerationMethod" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="PmoHeader" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="StageReadCounts" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="ReadCountsByStageForTarget" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="ReadCountsByStageForExperimentalSample" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="ReadCountsByStage" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="PortableMicrohaplotypeObject" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="ProjectInfo" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SpecimenInfo" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="BioinformaticsRunInfo" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="PmoGenerationMethod" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PmoHeader" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="StageReadCounts" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="ReadCountsByStageForTarget" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="ReadCountsByStageForExperimentalSample" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="ReadCountsByStage" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="PortableMicrohaplotypeObject" sheetId="31" state="visible" r:id="rId31"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -858,12 +859,12 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>extraction_plate_info</t>
+          <t>library_prep_plate_info</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>sequencing_prep_plate_info</t>
+          <t>qpcr_parasite_density_info</t>
         </is>
       </c>
     </row>
@@ -904,12 +905,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>forward_primers</t>
+          <t>forward_primer</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>reverse_primers</t>
+          <t>reverse_primer</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1035,6 +1036,280 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>density_method</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>parasite_density</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>date_measured</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>density_method_comments</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>project_description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>project_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>project_contributors</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>project_collector_chief_scientist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>BioProject_accession</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Y1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>specimen_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>specimen_taxon_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>host_subject_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>host_taxon_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>alternate_identifiers</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>host_sex</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>microscopy_parasite_density_info</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>collection_date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>host_age</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>collection_country</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>geo_admin1</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>geo_admin2</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>geo_admin3</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>lat_lon</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>specimen_store_loc</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>specimen_collect_device</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>specimen_type</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>project_id</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>specimen_comments</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>travel_out_six_month</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>storage_plate_info</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>env_medium</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>env_local_scale</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>env_broad_scale</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>drug_usage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bioinformatics_methods_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>run_date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>bioinformatics_run_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1046,172 +1321,385 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>method</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>density</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Z1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>specimen_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>specimen_taxon_id</t>
+          <t>program_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>program_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>pmo_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>creation_date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>host_subject_id</t>
+          <t>generation_method</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>read_count</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>stage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>target_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>stages</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>experiment_sample_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>total_raw_count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>read_counts_for_targets</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>panel_targets</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>reaction_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bioinformatics_run_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>read_counts_by_experimental_sample_by_stage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>experiment_info</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>specimen_info</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequencing_info</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>host_taxon_id</t>
+          <t>panel_info</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>alternate_identifiers</t>
+          <t>target_info</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>host_sex</t>
+          <t>targeted_genomes</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>parasite_density_info</t>
+          <t>microhaplotypes_info</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>collection_date</t>
+          <t>bioinformatics_methods_info</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>host_age</t>
+          <t>bioinformatics_run_info</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>collection_country</t>
+          <t>microhaplotypes_detected</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>geo_admin1</t>
+          <t>project_info</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>geo_admin2</t>
+          <t>pmo_header</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>geo_admin3</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>lat_lon</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>collector_chief_scientist</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>specimen_store_loc</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>specimen_collect_device</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>specimen_type</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>project_name</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>specimen_comments</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>travel_out_six_month</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>plate_info</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>env_medium</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>env_local_scale</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>env_broad_scale</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>drug_usage</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>read_counts_by_stage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>reactions</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>panel_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>seq</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>microhaplotype_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>quality</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pseudocigar</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>masking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>alt_annotations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1228,26 +1716,88 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>bioinformatics_methods_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>run_date</t>
+          <t>seq_start</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>seq_segment_size</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>bioinformatics_run_name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>replacement_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>targets</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>target_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>microhaplotypes</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mhap_location</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1264,494 +1814,11 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>program_version</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>program_name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>pmo_version</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>creation_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>generation_method</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>read_count</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>stage</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>target_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>stages</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>experiment_sample_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>total_raw_count</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>read_counts_for_targets</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>bioinformatics_run_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>read_counts_by_experimental_sample_by_stage</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>panel_targets</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>reaction_name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>experiment_info</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>specimen_info</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>sequencing_info</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>panel_info</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>target_info</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>targeted_genomes</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>microhaplotypes_info</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>bioinformatics_methods_info</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>bioinformatics_run_info</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>microhaplotypes_detected</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>pmo_header</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>read_counts_by_stage</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>reactions</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>panel_name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>seq</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>microhaplotype_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>quality</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>pseudocigar</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>masking</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>alt_annotations</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>seq_start</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>seq_segment_size</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>replacement_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>targets</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>target_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>microhaplotypes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bioinformatics_run_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>experiment_samples</t>
         </is>
       </c>

</xml_diff>